<commit_message>
Update PT Emergency Medicine Case Study.xlsx
Added a second fake case to csv tab and case tab
</commit_message>
<xml_diff>
--- a/data/PT Emergency Medicine Case Study.xlsx
+++ b/data/PT Emergency Medicine Case Study.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsimo\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C12954-FB33-4D9B-98E0-196154F2A344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Databases" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Default Labs  Interventions" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="DDx" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Case Info" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="CSV Case Info" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="GoalsTasks" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Flow chart" sheetId="7" r:id="rId10"/>
+    <sheet name="Databases" sheetId="1" r:id="rId1"/>
+    <sheet name="Default Labs  Interventions" sheetId="2" r:id="rId2"/>
+    <sheet name="DDx" sheetId="3" r:id="rId3"/>
+    <sheet name="Case Info" sheetId="4" r:id="rId4"/>
+    <sheet name="CSV Case Info" sheetId="5" r:id="rId5"/>
+    <sheet name="GoalsTasks" sheetId="6" r:id="rId6"/>
+    <sheet name="Flow chart" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="772">
   <si>
     <t>v1 11/20/19</t>
   </si>
@@ -2318,57 +2327,167 @@
   </si>
   <si>
     <t>Grading screen</t>
+  </si>
+  <si>
+    <t>Fak E. Case</t>
+  </si>
+  <si>
+    <t>winky eyes</t>
+  </si>
+  <si>
+    <t>Jimmy Simonse</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>jsimonse9@gmail.com</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>2 kg</t>
+  </si>
+  <si>
+    <t>A dark and shady history 1</t>
+  </si>
+  <si>
+    <t>A darker and shadier history 2</t>
+  </si>
+  <si>
+    <t>Cat cuddles</t>
+  </si>
+  <si>
+    <t>Adderol</t>
+  </si>
+  <si>
+    <t>Vodka</t>
+  </si>
+  <si>
+    <t>Wears oversized pants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No rhinoceruses
+</t>
+  </si>
+  <si>
+    <t>Ny algae</t>
+  </si>
+  <si>
+    <t>Ready to diffuse</t>
+  </si>
+  <si>
+    <t>Vampire bites</t>
+  </si>
+  <si>
+    <t>Brusing on nose hairs</t>
+  </si>
+  <si>
+    <t>Constantly drinks vodka</t>
+  </si>
+  <si>
+    <t>Anxious about clowns</t>
+  </si>
+  <si>
+    <t>Paper like thinness</t>
+  </si>
+  <si>
+    <t>pettasatus</t>
+  </si>
+  <si>
+    <t>Supple nose and left ear</t>
+  </si>
+  <si>
+    <t>Normal S1, S2, S3</t>
+  </si>
+  <si>
+    <t>Has two lungs</t>
+  </si>
+  <si>
+    <t>Has two arms</t>
+  </si>
+  <si>
+    <t>Dry Eyes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2376,7 +2495,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2398,115 +2517,109 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="29">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>61</xdr:col>
@@ -2517,11 +2630,17 @@
     <xdr:ext cx="3152775" cy="1447800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="2" name="image1.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2538,20 +2657,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -2741,25 +2848,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AB60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.0"/>
-    <col customWidth="1" min="2" max="2" width="19.29"/>
-    <col customWidth="1" min="4" max="4" width="17.43"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2782,7 +2892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -2820,7 +2930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -2849,7 +2959,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -2884,7 +2994,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -2904,7 +3014,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
@@ -2942,7 +3052,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>177</v>
       </c>
@@ -2983,12 +3093,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>191</v>
       </c>
@@ -3011,40 +3121,40 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>268</v>
       </c>
@@ -3052,7 +3162,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>272</v>
       </c>
@@ -3136,7 +3246,7 @@
       </c>
       <c r="AB52" s="1"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>325</v>
       </c>
@@ -3204,32 +3314,33 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
       <c r="L60" s="1" t="s">
         <v>164</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="29.29"/>
-    <col customWidth="1" min="3" max="3" width="18.86"/>
-    <col customWidth="1" min="6" max="6" width="17.57"/>
+    <col min="2" max="2" width="29.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3243,7 +3354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3272,7 +3383,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>55</v>
       </c>
@@ -3322,7 +3433,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
@@ -3399,7 +3510,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
@@ -3446,7 +3557,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>101</v>
       </c>
@@ -3484,7 +3595,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>110</v>
       </c>
@@ -3522,7 +3633,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>119</v>
       </c>
@@ -3551,7 +3662,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" ht="17.25" customHeight="1">
+    <row r="9" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>127</v>
       </c>
@@ -3571,7 +3682,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>133</v>
       </c>
@@ -3591,7 +3702,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
         <v>141</v>
       </c>
@@ -3605,7 +3716,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>144</v>
       </c>
@@ -3622,7 +3733,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>151</v>
       </c>
@@ -3633,7 +3744,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>155</v>
       </c>
@@ -3650,7 +3761,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>160</v>
       </c>
@@ -3670,7 +3781,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>165</v>
       </c>
@@ -3687,7 +3798,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
@@ -3737,7 +3848,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>172</v>
       </c>
@@ -3802,7 +3913,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="J23" s="1" t="s">
         <v>212</v>
       </c>
@@ -3831,7 +3942,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="M24" s="1" t="s">
         <v>224</v>
       </c>
@@ -3854,7 +3965,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="M25" s="1" t="s">
         <v>237</v>
       </c>
@@ -3877,7 +3988,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="M26" s="1" t="s">
         <v>245</v>
       </c>
@@ -3900,7 +4011,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="M27" s="1" t="s">
         <v>252</v>
       </c>
@@ -3923,7 +4034,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S28" s="1" t="s">
         <v>260</v>
       </c>
@@ -3940,7 +4051,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S29" s="1" t="s">
         <v>136</v>
       </c>
@@ -3954,7 +4065,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S30" s="1" t="s">
         <v>276</v>
       </c>
@@ -3962,7 +4073,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S31" s="1" t="s">
         <v>282</v>
       </c>
@@ -3970,7 +4081,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:27" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S32" s="1" t="s">
         <v>286</v>
       </c>
@@ -3978,7 +4089,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="19:21" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S33" s="1" t="s">
         <v>290</v>
       </c>
@@ -3986,12 +4097,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="19:21" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S34" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="19:21" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S35" s="1" t="s">
         <v>299</v>
       </c>
@@ -4002,7 +4113,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="19:21" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S36" s="1" t="s">
         <v>307</v>
       </c>
@@ -4013,7 +4124,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="19:21" ht="12.5" x14ac:dyDescent="0.25">
       <c r="S37" s="1" t="s">
         <v>312</v>
       </c>
@@ -4025,31 +4136,32 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.71"/>
-    <col customWidth="1" min="2" max="2" width="26.86"/>
-    <col customWidth="1" min="3" max="3" width="41.57"/>
-    <col customWidth="1" min="4" max="4" width="36.57"/>
-    <col customWidth="1" min="5" max="5" width="34.14"/>
-    <col customWidth="1" min="6" max="6" width="30.43"/>
-    <col customWidth="1" min="7" max="7" width="33.14"/>
-    <col customWidth="1" min="8" max="8" width="24.29"/>
+    <col min="1" max="1" width="31.7265625" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="3" max="3" width="41.54296875" customWidth="1"/>
+    <col min="4" max="4" width="36.54296875" customWidth="1"/>
+    <col min="5" max="5" width="34.08984375" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" customWidth="1"/>
+    <col min="7" max="7" width="33.08984375" customWidth="1"/>
+    <col min="8" max="8" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -4061,7 +4173,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -4071,7 +4183,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -4095,7 +4207,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>115</v>
       </c>
@@ -4119,7 +4231,7 @@
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>149</v>
       </c>
@@ -4143,7 +4255,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>161</v>
       </c>
@@ -4167,7 +4279,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>183</v>
       </c>
@@ -4191,7 +4303,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>192</v>
       </c>
@@ -4215,7 +4327,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>222</v>
       </c>
@@ -4239,7 +4351,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>238</v>
       </c>
@@ -4263,7 +4375,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>253</v>
       </c>
@@ -4287,7 +4399,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>270</v>
       </c>
@@ -4311,7 +4423,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>189</v>
       </c>
@@ -4333,7 +4445,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>314</v>
       </c>
@@ -4353,7 +4465,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>326</v>
       </c>
@@ -4373,7 +4485,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>335</v>
       </c>
@@ -4393,7 +4505,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>349</v>
       </c>
@@ -4415,7 +4527,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -4435,7 +4547,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -4455,7 +4567,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -4475,7 +4587,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>371</v>
       </c>
@@ -4497,7 +4609,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>377</v>
       </c>
@@ -4517,7 +4629,7 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>382</v>
       </c>
@@ -4539,7 +4651,7 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>388</v>
       </c>
@@ -4559,7 +4671,7 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>393</v>
       </c>
@@ -4581,7 +4693,7 @@
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>399</v>
       </c>
@@ -4603,7 +4715,7 @@
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>405</v>
       </c>
@@ -4625,7 +4737,7 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>411</v>
       </c>
@@ -4643,7 +4755,7 @@
       </c>
       <c r="H28" s="7"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>415</v>
       </c>
@@ -4661,7 +4773,7 @@
       </c>
       <c r="H29" s="7"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>419</v>
       </c>
@@ -4681,7 +4793,7 @@
       </c>
       <c r="H30" s="7"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>223</v>
       </c>
@@ -4705,7 +4817,7 @@
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>428</v>
       </c>
@@ -4729,7 +4841,7 @@
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>435</v>
       </c>
@@ -4753,7 +4865,7 @@
       </c>
       <c r="H33" s="7"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>314</v>
       </c>
@@ -4777,7 +4889,7 @@
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>448</v>
       </c>
@@ -4799,7 +4911,7 @@
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>156</v>
       </c>
@@ -4823,7 +4935,7 @@
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>189</v>
       </c>
@@ -4847,7 +4959,7 @@
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>342</v>
       </c>
@@ -4871,7 +4983,7 @@
       </c>
       <c r="H38" s="7"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
         <v>377</v>
       </c>
@@ -4895,7 +5007,7 @@
       </c>
       <c r="H39" s="7"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>382</v>
       </c>
@@ -4919,7 +5031,7 @@
       </c>
       <c r="H40" s="7"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>388</v>
       </c>
@@ -4941,7 +5053,7 @@
       <c r="G41" s="5"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>393</v>
       </c>
@@ -4963,7 +5075,7 @@
       <c r="G42" s="5"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>399</v>
       </c>
@@ -4983,7 +5095,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>532</v>
       </c>
@@ -5003,7 +5115,7 @@
       <c r="G44" s="5"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>411</v>
       </c>
@@ -5021,7 +5133,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A46" s="16" t="s">
         <v>415</v>
       </c>
@@ -5041,7 +5153,7 @@
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>419</v>
       </c>
@@ -5061,7 +5173,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>223</v>
       </c>
@@ -5081,7 +5193,7 @@
       <c r="G48" s="5"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>428</v>
       </c>
@@ -5099,7 +5211,7 @@
       <c r="G49" s="5"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>435</v>
       </c>
@@ -5121,7 +5233,7 @@
       <c r="G50" s="5"/>
       <c r="H50" s="7"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>314</v>
       </c>
@@ -5143,7 +5255,7 @@
       <c r="G51" s="5"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>448</v>
       </c>
@@ -5163,7 +5275,7 @@
       <c r="G52" s="5"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>156</v>
       </c>
@@ -5183,7 +5295,7 @@
       <c r="G53" s="5"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>189</v>
       </c>
@@ -5203,7 +5315,7 @@
       <c r="G54" s="5"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>342</v>
       </c>
@@ -5223,7 +5335,7 @@
       <c r="G55" s="5"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="15" t="s">
         <v>616</v>
@@ -5241,7 +5353,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
         <v>632</v>
       </c>
@@ -5259,7 +5371,7 @@
       <c r="G57" s="5"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>273</v>
       </c>
@@ -5277,7 +5389,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="7"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>641</v>
       </c>
@@ -5295,7 +5407,7 @@
       <c r="G59" s="5"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>645</v>
       </c>
@@ -5311,7 +5423,7 @@
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>646</v>
       </c>
@@ -5329,7 +5441,7 @@
       <c r="G61" s="5"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>601</v>
       </c>
@@ -5347,7 +5459,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>195</v>
       </c>
@@ -5365,7 +5477,7 @@
       <c r="G63" s="5"/>
       <c r="H63" s="7"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>364</v>
       </c>
@@ -5383,7 +5495,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="7"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
         <v>659</v>
       </c>
@@ -5401,7 +5513,7 @@
       <c r="G65" s="5"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>356</v>
       </c>
@@ -5419,7 +5531,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>665</v>
       </c>
@@ -5435,7 +5547,7 @@
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>668</v>
       </c>
@@ -5451,7 +5563,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="17" t="s">
@@ -5465,7 +5577,7 @@
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="17" t="s">
@@ -5479,7 +5591,7 @@
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="17" t="s">
@@ -5491,7 +5603,7 @@
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7" t="s">
@@ -5503,7 +5615,7 @@
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7" t="s">
@@ -5515,7 +5627,7 @@
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="17" t="s">
@@ -5527,7 +5639,7 @@
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7" t="s">
@@ -5539,7 +5651,7 @@
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7" t="s">
@@ -5551,7 +5663,7 @@
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7" t="s">
@@ -5563,7 +5675,7 @@
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7" t="s">
@@ -5575,7 +5687,7 @@
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7" t="s">
@@ -5587,7 +5699,7 @@
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7" t="s">
@@ -5599,7 +5711,7 @@
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7" t="s">
@@ -5611,7 +5723,7 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -5621,7 +5733,7 @@
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -5631,7 +5743,7 @@
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -5641,7 +5753,7 @@
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -5651,7 +5763,7 @@
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -5661,7 +5773,7 @@
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -5671,7 +5783,7 @@
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -5682,21 +5794,24 @@
       <c r="H88" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:BX7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:AY3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>554</v>
       </c>
@@ -5875,9 +5990,9 @@
       <c r="BW1" s="1"/>
       <c r="BX1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>451</v>
@@ -5889,10 +6004,10 @@
         <v>455</v>
       </c>
       <c r="E2" s="24">
-        <v>43780.0</v>
+        <v>43780</v>
       </c>
       <c r="F2" s="24">
-        <v>43780.0</v>
+        <v>43780</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>480</v>
@@ -5904,7 +6019,7 @@
         <v>482</v>
       </c>
       <c r="L2" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>485</v>
@@ -5982,19 +6097,19 @@
         <v>518</v>
       </c>
       <c r="AO2" s="1">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="AP2" s="1">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="AQ2" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="AR2" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="AS2" s="1">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="AT2" s="1" t="s">
         <v>378</v>
@@ -6036,37 +6151,187 @@
       <c r="BW2" s="1"/>
       <c r="BX2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>744</v>
+      </c>
+      <c r="C3" t="s">
+        <v>745</v>
+      </c>
+      <c r="D3" t="s">
+        <v>746</v>
+      </c>
+      <c r="E3" s="24">
+        <v>43792</v>
+      </c>
+      <c r="F3" s="24">
+        <v>43792</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>747</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>748</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>749</v>
+      </c>
+      <c r="L3">
+        <v>937</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>750</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>751</v>
+      </c>
+      <c r="O3" s="26" t="s">
+        <v>752</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>754</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>755</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>756</v>
+      </c>
+      <c r="T3" s="26" t="s">
+        <v>757</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>758</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="W3" s="26" t="s">
+        <v>759</v>
+      </c>
+      <c r="X3" s="26" t="s">
+        <v>760</v>
+      </c>
+      <c r="Y3" s="26" t="s">
+        <v>761</v>
+      </c>
+      <c r="Z3" s="26" t="s">
+        <v>762</v>
+      </c>
+      <c r="AA3" s="26" t="s">
+        <v>763</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="AC3" s="26" t="s">
+        <v>765</v>
+      </c>
+      <c r="AD3" s="26" t="s">
+        <v>766</v>
+      </c>
+      <c r="AE3" s="26" t="s">
+        <v>767</v>
+      </c>
+      <c r="AF3" s="26" t="s">
+        <v>768</v>
+      </c>
+      <c r="AG3" s="26" t="s">
+        <v>769</v>
+      </c>
+      <c r="AH3" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="AI3" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="AJ3" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="AK3" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="AL3" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="AM3" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="AN3">
+        <v>37</v>
+      </c>
+      <c r="AO3">
+        <v>129</v>
+      </c>
+      <c r="AP3">
+        <v>69</v>
+      </c>
+      <c r="AQ3">
+        <v>99</v>
+      </c>
+      <c r="AR3">
+        <v>19</v>
+      </c>
+      <c r="AS3">
+        <v>98</v>
+      </c>
+      <c r="AT3" s="26" t="s">
+        <v>771</v>
+      </c>
+      <c r="AU3" s="26" t="s">
+        <v>620</v>
+      </c>
+      <c r="AV3" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="AW3" s="26" t="s">
+        <v>623</v>
+      </c>
+      <c r="AX3" s="26" t="s">
+        <v>624</v>
+      </c>
       <c r="AY3" s="1" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AK7" s="1" t="s">
         <v>164</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="BK1"/>
+    <hyperlink ref="BK1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{8F463A94-B979-4D46-8383-60405AA028D1}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AY2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>451</v>
@@ -6078,10 +6343,10 @@
         <v>455</v>
       </c>
       <c r="E1" s="24">
-        <v>43780.0</v>
+        <v>43780</v>
       </c>
       <c r="F1" s="24">
-        <v>43780.0</v>
+        <v>43780</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>480</v>
@@ -6093,7 +6358,7 @@
         <v>482</v>
       </c>
       <c r="L1" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>485</v>
@@ -6171,19 +6436,19 @@
         <v>518</v>
       </c>
       <c r="AO1" s="1">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="AP1" s="1">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="AQ1" s="1">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="AR1" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="AS1" s="1">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>378</v>
@@ -6204,26 +6469,179 @@
         <v>528</v>
       </c>
     </row>
+    <row r="2" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C2" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2" t="s">
+        <v>746</v>
+      </c>
+      <c r="E2" s="24">
+        <v>43792</v>
+      </c>
+      <c r="F2" s="24">
+        <v>43792</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>747</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>748</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>749</v>
+      </c>
+      <c r="L2">
+        <v>937</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>750</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>751</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>752</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>753</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>754</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>755</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>756</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>757</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>758</v>
+      </c>
+      <c r="V2" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="W2" s="26" t="s">
+        <v>759</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>760</v>
+      </c>
+      <c r="Y2" s="26" t="s">
+        <v>761</v>
+      </c>
+      <c r="Z2" s="26" t="s">
+        <v>762</v>
+      </c>
+      <c r="AA2" s="26" t="s">
+        <v>763</v>
+      </c>
+      <c r="AB2" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="AC2" s="26" t="s">
+        <v>765</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>766</v>
+      </c>
+      <c r="AE2" s="26" t="s">
+        <v>767</v>
+      </c>
+      <c r="AF2" s="26" t="s">
+        <v>768</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>769</v>
+      </c>
+      <c r="AH2" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="AI2" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="AJ2" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="AK2" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="AL2" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="AM2" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="AN2">
+        <v>37</v>
+      </c>
+      <c r="AO2">
+        <v>129</v>
+      </c>
+      <c r="AP2">
+        <v>69</v>
+      </c>
+      <c r="AQ2">
+        <v>99</v>
+      </c>
+      <c r="AR2">
+        <v>19</v>
+      </c>
+      <c r="AS2">
+        <v>98</v>
+      </c>
+      <c r="AT2" s="26" t="s">
+        <v>771</v>
+      </c>
+      <c r="AU2" s="26" t="s">
+        <v>620</v>
+      </c>
+      <c r="AV2" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="AW2" s="26" t="s">
+        <v>623</v>
+      </c>
+      <c r="AX2" s="26" t="s">
+        <v>624</v>
+      </c>
+      <c r="AY2" s="7" t="s">
+        <v>699</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{3E8E5F80-52F8-4CD0-A0DF-95AC63DD0161}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.57"/>
-    <col customWidth="1" min="4" max="4" width="19.14"/>
+    <col min="1" max="1" width="32.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>669</v>
       </c>
@@ -6231,7 +6649,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>674</v>
       </c>
@@ -6242,95 +6660,96 @@
         <v>677</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>690</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A3:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.14"/>
-    <col customWidth="1" min="2" max="2" width="5.14"/>
-    <col customWidth="1" min="3" max="3" width="39.14"/>
-    <col customWidth="1" min="4" max="4" width="5.57"/>
-    <col customWidth="1" min="5" max="5" width="54.71"/>
-    <col customWidth="1" min="6" max="6" width="4.43"/>
-    <col customWidth="1" min="7" max="7" width="27.0"/>
-    <col customWidth="1" min="8" max="8" width="5.71"/>
-    <col customWidth="1" min="9" max="9" width="29.43"/>
-    <col customWidth="1" min="10" max="10" width="5.71"/>
-    <col customWidth="1" min="11" max="11" width="31.29"/>
+    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="5.08984375" customWidth="1"/>
+    <col min="3" max="3" width="39.08984375" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" customWidth="1"/>
+    <col min="5" max="5" width="54.7265625" customWidth="1"/>
+    <col min="6" max="6" width="4.453125" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="5.7265625" customWidth="1"/>
+    <col min="9" max="9" width="29.453125" customWidth="1"/>
+    <col min="10" max="10" width="5.7265625" customWidth="1"/>
+    <col min="11" max="11" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="18" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>708</v>
       </c>
@@ -6347,7 +6766,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>198</v>
       </c>
@@ -6376,7 +6795,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>709</v>
       </c>
@@ -6390,7 +6809,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>709</v>
       </c>
@@ -6404,7 +6823,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>709</v>
       </c>
@@ -6415,7 +6834,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>715</v>
       </c>
@@ -6429,7 +6848,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
         <v>709</v>
       </c>
@@ -6443,7 +6862,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>709</v>
       </c>
@@ -6451,7 +6870,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>727</v>
       </c>
@@ -6471,7 +6890,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H14" s="18" t="s">
         <v>715</v>
       </c>
@@ -6480,7 +6899,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H15" s="1" t="s">
         <v>709</v>
       </c>
@@ -6491,32 +6910,32 @@
         <v>733</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K16" s="18" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K17" s="18" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K18" s="1" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K19" s="1" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="4:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K20" s="1" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="4:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
         <v>709</v>
       </c>
@@ -6533,7 +6952,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="4:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
         <v>709</v>
       </c>
@@ -6557,6 +6976,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>